<commit_message>
Added collapsible tree example and version 1 of app
</commit_message>
<xml_diff>
--- a/test-data.xlsx
+++ b/test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/peter_zajdel_ucalgary_ca/Documents/Peter/_Personal/_Programming/R/Projects/r-first-shiny-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabby\Desktop\Life\R Conference\Shiny\r-first-shiny-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A53DC789-2F6C-4485-8E6F-61B225519DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF971C6-791F-4319-BA7D-072AD6EE49CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A3BB06BE-21DD-4533-A165-A4F2A4DCE8C0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{A3BB06BE-21DD-4533-A165-A4F2A4DCE8C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -464,16 +462,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E29536-F54C-4C6F-BF04-7AB71E0120DC}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,7 +585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,7 +641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,7 +655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>